<commit_message>
tidycode make sure gla mca working change download names and neaten up columns update dat table update data text to qirk wqork qual plus 3
</commit_message>
<xml_diff>
--- a/Data/3-1_DataTable/221004DataTable.xlsx
+++ b/Data/3-1_DataTable/221004DataTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\8_DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjames2\OneDrive - Department for Education\Documents\RProjects\lsip_dashboard\Data\3-1_DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3F521F-D9AA-4EF7-9FF3-03C9CC650378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2860D04-B9BE-4882-B709-F6C7125360C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -59,15 +59,6 @@
     <t>To be announced</t>
   </si>
   <si>
-    <t>Employment rates</t>
-  </si>
-  <si>
-    <t>Employment share by occupation</t>
-  </si>
-  <si>
-    <t>Further education and skills achievements</t>
-  </si>
-  <si>
     <t>Further education and skills achievements by sector subject area</t>
   </si>
   <si>
@@ -80,9 +71,6 @@
     <t>Aug 2021 – Jul 2022 (24/11/22)</t>
   </si>
   <si>
-    <t>Aug 2022 – Jan 2023 (Mar 23)</t>
-  </si>
-  <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/cae2bcbb-e385-4da7-8d7b-08dacbbccc68'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
@@ -110,9 +98,6 @@
     <t>Enterprises by employment size band</t>
   </si>
   <si>
-    <t>Enterprises by employment size band and industry</t>
-  </si>
-  <si>
     <t>Dec 2020 - Dec 2021 (17/11/22)</t>
   </si>
   <si>
@@ -159,6 +144,21 @@
   </si>
   <si>
     <t>&lt;a href='https://www.gov.uk/government/publications/labour-market-and-skills-projections-2020-to-2035'&gt;Skills Imperative 2035&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Further education and skills achievements and participation by provision, level and age group</t>
+  </si>
+  <si>
+    <t>Employment by occupation</t>
+  </si>
+  <si>
+    <t>Employment volumes</t>
+  </si>
+  <si>
+    <t>Enterprises by employment industry</t>
+  </si>
+  <si>
+    <t>Aug 2022 – Jul 2023 (Nov 23)</t>
   </si>
 </sst>
 </file>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,7 +572,7 @@
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -581,26 +581,26 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -609,130 +609,130 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -740,13 +740,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>

</xml_diff>